<commit_message>
New k values from ICES report
</commit_message>
<xml_diff>
--- a/Data/DR_Stocks/Advice Sheets/2022/stock_metadata_refpts.xlsx
+++ b/Data/DR_Stocks/Advice Sheets/2022/stock_metadata_refpts.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefas-my.sharepoint.com/personal/peter_kidd_cefas_gov_uk/Documents/Projects/C8503B/PhD/DATRAS/Spatial Indicator R Project/Stocks/Advice Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefas-my.sharepoint.com/personal/peter_kidd_cefas_gov_uk/Documents/Projects/C8503B/PhD/SpatIndAssess(GIT)/SpatIndAssess/Data/DR_Stocks/Advice Sheets/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{A8FB5902-299E-49A2-BD1E-0FEA1BCA3EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{245C175E-F614-4D10-A931-FFFCBD355124}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{A8FB5902-299E-49A2-BD1E-0FEA1BCA3EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CE26B89-7A03-44D6-AB0F-F124A9D81786}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F2B49E6A-08D5-481B-9D34-DE9AC72A6B55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F2B49E6A-08D5-481B-9D34-DE9AC72A6B55}"/>
   </bookViews>
   <sheets>
     <sheet name="stk_metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="stk_refpts" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="spcs_info" sheetId="4" r:id="rId2"/>
+    <sheet name="stk_refpts" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stk_metadata!$A$1:$N$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="172">
   <si>
     <t>stk_id</t>
   </si>
@@ -386,13 +387,205 @@
   </si>
   <si>
     <t>IE-IGFS</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Ecoregions</t>
+  </si>
+  <si>
+    <t>ICES Areas</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>bll.27.3a47de</t>
+  </si>
+  <si>
+    <t>brill (Scophthalmus rhombus)</t>
+  </si>
+  <si>
+    <t>SPiCT assessment</t>
+  </si>
+  <si>
+    <t>Celtic Seas, Greater North Sea</t>
+  </si>
+  <si>
+    <t>North Sea, Skagerrak and Kattegat, English Channel</t>
+  </si>
+  <si>
+    <t>Subarea 4 and divisions 3.a and 7.d–e</t>
+  </si>
+  <si>
+    <t>Benthic</t>
+  </si>
+  <si>
+    <t>Medium demersal</t>
+  </si>
+  <si>
+    <t>demersal piscivore</t>
+  </si>
+  <si>
+    <t>Flatfish</t>
+  </si>
+  <si>
+    <t>cod (Gadus morhua)</t>
+  </si>
+  <si>
+    <t>Age-based analytical assessment (SAM)</t>
+  </si>
+  <si>
+    <t>Greater North Sea</t>
+  </si>
+  <si>
+    <t>North Sea, eastern English Channel, Skagerrak</t>
+  </si>
+  <si>
+    <t>Subarea 4, Division 7.d, and Subdivision 20</t>
+  </si>
+  <si>
+    <t>Demersal</t>
+  </si>
+  <si>
+    <t>Large benthopelagic</t>
+  </si>
+  <si>
+    <t>Gadoid</t>
+  </si>
+  <si>
+    <t>haddock (Melanogrammus aeglefinus)</t>
+  </si>
+  <si>
+    <t>North Sea, West of Scotland, Skagerrak</t>
+  </si>
+  <si>
+    <t>Subarea 4, Division 6.a, and Subdivision 20</t>
+  </si>
+  <si>
+    <t>plaice (Pleuronectes platessa)</t>
+  </si>
+  <si>
+    <t>Age-based analytical assessment (Aart and Poos)</t>
+  </si>
+  <si>
+    <t>Eastern English Channel</t>
+  </si>
+  <si>
+    <t>Division 7.d</t>
+  </si>
+  <si>
+    <t>Large demersal</t>
+  </si>
+  <si>
+    <t>demersal benthivore</t>
+  </si>
+  <si>
+    <t>North Sea, Skagerrak</t>
+  </si>
+  <si>
+    <t>Subarea 4 and Subdivision 20</t>
+  </si>
+  <si>
+    <t>saithe (Pollachius virens)</t>
+  </si>
+  <si>
+    <t>Celtic Seas, Faroes, Greater North Sea</t>
+  </si>
+  <si>
+    <t>North Sea, Rockall and West of Scotland, Skagerrak and Kattegat</t>
+  </si>
+  <si>
+    <t>Subareas 4 and 6, and in Division 3.a</t>
+  </si>
+  <si>
+    <t>sole (Solea solea)</t>
+  </si>
+  <si>
+    <t>North Sea</t>
+  </si>
+  <si>
+    <t>Subarea 4</t>
+  </si>
+  <si>
+    <t>turbot (Scophthalmus maximus)</t>
+  </si>
+  <si>
+    <t>whiting (Merlangius merlangus)</t>
+  </si>
+  <si>
+    <t>North Sea and eastern English Channel</t>
+  </si>
+  <si>
+    <t>Subarea 4 and Division 7.d</t>
+  </si>
+  <si>
+    <t>Medium benthopelagic</t>
+  </si>
+  <si>
+    <t>witch (Glyptocephalus cynoglossus)</t>
+  </si>
+  <si>
+    <t>North Sea, Skagerrak and Kattegat, eastern English Channel</t>
+  </si>
+  <si>
+    <t>Subarea 4 and divisions 3.a and 7.d</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>FisheriesGuild</t>
+  </si>
+  <si>
+    <t>SizeGuild</t>
+  </si>
+  <si>
+    <t>TrophicGuild</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>AssessmentType</t>
+  </si>
+  <si>
+    <t>AdviceYear</t>
+  </si>
+  <si>
+    <t>StockID</t>
+  </si>
+  <si>
+    <t>DataCategory</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>linf</t>
+  </si>
+  <si>
+    <t>l50</t>
+  </si>
+  <si>
+    <t>a50</t>
+  </si>
+  <si>
+    <t>t0</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +595,20 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -433,11 +640,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1730,7 +1939,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BTS</c:v>
+                  <c:v>IBTS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1763,7 +1972,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1783,7 +1992,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BTS-Isis</c:v>
+                  <c:v>SNS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1816,7 +2025,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1836,7 +2045,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FR-GFS</c:v>
+                  <c:v>BTS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1869,7 +2078,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1889,7 +2098,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FR-YFS</c:v>
+                  <c:v>BTS-Isis</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1922,7 +2131,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1942,7 +2151,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>IBTS</c:v>
+                  <c:v>SWC-IBTS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1975,7 +2184,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1995,7 +2204,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>IGFS</c:v>
+                  <c:v>SCOWCGFS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2028,7 +2237,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2048,7 +2257,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SCOWCGFS</c:v>
+                  <c:v>UK-BTS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2083,7 +2292,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2103,7 +2312,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SNS</c:v>
+                  <c:v>YFS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2138,7 +2347,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2158,7 +2367,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SWC-IBTS</c:v>
+                  <c:v>FR-YFS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2193,7 +2402,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2213,7 +2422,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UK-BTS</c:v>
+                  <c:v>FR-GFS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2268,7 +2477,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>YFS</c:v>
+                  <c:v>IGFS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3090,16 +3299,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>387351</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>6351</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>768351</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>74931</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>244475</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>116206</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3699,7 +3908,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49A3D42E-6D97-4AFD-983C-4FC950976605}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49A3D42E-6D97-4AFD-983C-4FC950976605}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:M5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="14">
     <pivotField axis="axisPage" showAll="0">
@@ -3722,7 +3931,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
+    <pivotField axis="axisCol" dataField="1" showAll="0" sortType="descending">
       <items count="12">
         <item x="6"/>
         <item x="7"/>
@@ -3737,6 +3946,15 @@
         <item x="9"/>
         <item t="default"/>
       </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -3754,37 +3972,37 @@
   </colFields>
   <colItems count="12">
     <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
       <x/>
     </i>
     <i>
       <x v="1"/>
     </i>
     <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
+      <x v="8"/>
     </i>
     <i>
       <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
     </i>
     <i>
       <x v="9"/>
     </i>
     <i>
       <x v="10"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -4256,31 +4474,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237EF871-549E-4BB3-8241-1B75354C421D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.81640625" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.77734375" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4324,7 +4541,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -4362,7 +4579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4400,7 +4617,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4432,7 +4649,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4464,7 +4681,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4496,7 +4713,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -4528,7 +4745,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4560,7 +4777,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4592,7 +4809,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4624,7 +4841,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -4662,7 +4879,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -4700,7 +4917,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -4735,7 +4952,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -4773,7 +4990,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -4808,7 +5025,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -4843,7 +5060,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -4872,7 +5089,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -4901,7 +5118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -4939,7 +5156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -4971,7 +5188,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -5003,7 +5220,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -5032,7 +5249,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -5061,7 +5278,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -5090,7 +5307,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -5119,7 +5336,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -5148,7 +5365,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -5189,7 +5406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -5230,7 +5447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -5265,7 +5482,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -5300,7 +5517,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -5337,11 +5554,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:N31" xr:uid="{237EF871-549E-4BB3-8241-1B75354C421D}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="wit.27.3a47d"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N31">
       <sortCondition ref="A1:A31"/>
     </sortState>
@@ -5353,6 +5565,668 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A949D5-DEA6-481C-BF0D-9F5D23895FB7}">
+  <dimension ref="A1:S12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="43.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="56.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="37.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" t="s">
+        <v>166</v>
+      </c>
+      <c r="O1" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>169</v>
+      </c>
+      <c r="R1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="N2">
+        <v>3.01</v>
+      </c>
+      <c r="O2">
+        <v>58</v>
+      </c>
+      <c r="P2">
+        <v>31.3</v>
+      </c>
+      <c r="Q2">
+        <v>1.6</v>
+      </c>
+      <c r="R2">
+        <v>-0.27</v>
+      </c>
+      <c r="S2">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2022</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L3" t="s">
+        <v>129</v>
+      </c>
+      <c r="O3">
+        <v>123.1</v>
+      </c>
+      <c r="S3" s="4">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2022</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" t="s">
+        <v>128</v>
+      </c>
+      <c r="K4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L4" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="N4">
+        <v>2.96</v>
+      </c>
+      <c r="O4">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="P4" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>-0.36</v>
+      </c>
+      <c r="S4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K5" t="s">
+        <v>138</v>
+      </c>
+      <c r="L5" t="s">
+        <v>121</v>
+      </c>
+      <c r="M5">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="N5">
+        <v>2.9580000000000002</v>
+      </c>
+      <c r="O5">
+        <v>48</v>
+      </c>
+      <c r="P5">
+        <v>22.9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>171</v>
+      </c>
+      <c r="R5" t="s">
+        <v>171</v>
+      </c>
+      <c r="S5">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I6" t="s">
+        <v>118</v>
+      </c>
+      <c r="J6" t="s">
+        <v>137</v>
+      </c>
+      <c r="K6" t="s">
+        <v>138</v>
+      </c>
+      <c r="L6" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="N6">
+        <v>2.9580000000000002</v>
+      </c>
+      <c r="O6">
+        <v>48</v>
+      </c>
+      <c r="P6">
+        <v>22.9</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>171</v>
+      </c>
+      <c r="R6" t="s">
+        <v>171</v>
+      </c>
+      <c r="S6">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2022</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" t="s">
+        <v>137</v>
+      </c>
+      <c r="K7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" t="s">
+        <v>129</v>
+      </c>
+      <c r="O7">
+        <v>177.1</v>
+      </c>
+      <c r="S7" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2022</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L8" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8">
+        <v>39</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>2022</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="O9" s="4">
+        <v>39</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2022</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H10" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" t="s">
+        <v>137</v>
+      </c>
+      <c r="K10" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" t="s">
+        <v>121</v>
+      </c>
+      <c r="M10">
+        <v>1.49E-2</v>
+      </c>
+      <c r="N10">
+        <v>3.0790000000000002</v>
+      </c>
+      <c r="O10">
+        <v>66.7</v>
+      </c>
+      <c r="P10">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="Q10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S10">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2022</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" t="s">
+        <v>152</v>
+      </c>
+      <c r="K11" t="s">
+        <v>120</v>
+      </c>
+      <c r="L11" t="s">
+        <v>129</v>
+      </c>
+      <c r="M11">
+        <v>1.03E-2</v>
+      </c>
+      <c r="N11">
+        <v>2.395</v>
+      </c>
+      <c r="O11">
+        <v>38</v>
+      </c>
+      <c r="P11">
+        <v>28</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>171</v>
+      </c>
+      <c r="R11">
+        <v>-1.01</v>
+      </c>
+      <c r="S11">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2022</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" t="s">
+        <v>154</v>
+      </c>
+      <c r="H12" t="s">
+        <v>155</v>
+      </c>
+      <c r="I12" t="s">
+        <v>118</v>
+      </c>
+      <c r="J12" t="s">
+        <v>119</v>
+      </c>
+      <c r="K12" t="s">
+        <v>138</v>
+      </c>
+      <c r="L12" t="s">
+        <v>121</v>
+      </c>
+      <c r="O12">
+        <v>45.5</v>
+      </c>
+      <c r="S12" s="4">
+        <v>0.16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10449FC8-06F4-45FC-AC09-5C957788E9BA}">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -5360,15 +6234,15 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -5397,7 +6271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5426,7 +6300,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5455,7 +6329,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -5484,7 +6358,7 @@
         <v>0.23799999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -5513,7 +6387,7 @@
         <v>0.182</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -5542,7 +6416,7 @@
         <v>0.57599999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -5571,7 +6445,7 @@
         <v>0.311</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -5600,7 +6474,7 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -5626,7 +6500,7 @@
         <v>0.85599999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -5655,7 +6529,7 @@
         <v>0.47299999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -5689,53 +6563,53 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5431229-2C30-4724-A983-12640431697C}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5743,79 +6617,79 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>50</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" t="s">
         <v>46</v>
       </c>
-      <c r="E4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" t="s">
-        <v>68</v>
       </c>
       <c r="M4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>97</v>
       </c>
       <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>11</v>
-      </c>
-      <c r="G5">
+      <c r="J5">
         <v>1</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
       </c>
       <c r="K5">
         <v>1</v>

</xml_diff>